<commit_message>
Add new NEM case
Added new NEM case
Additional check to avoid 0 values for MUT & MDT of generators
</commit_message>
<xml_diff>
--- a/data/HVDC parameters.xlsx
+++ b/data/HVDC parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hergun/.julia/dev/StorageHVDC/test/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hergun/.julia/dev/ISPhvdc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8E3F8-0969-064B-911B-4BE63D7B028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80C78D0-818F-A643-A03B-077D71B4B23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="-21100" windowWidth="35080" windowHeight="21100" xr2:uid="{F1BAE6B8-B733-FC4B-AC64-50856C17FAC8}"/>
+    <workbookView xWindow="-11820" yWindow="-28300" windowWidth="51180" windowHeight="28300" xr2:uid="{F1BAE6B8-B733-FC4B-AC64-50856C17FAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcualtions" sheetId="1" r:id="rId1"/>
@@ -5604,7 +5604,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5771,6 +5771,10 @@
         <f xml:space="preserve"> L5 * SIN( ATAN(L2))</f>
         <v>7.4969406484552108</v>
       </c>
+      <c r="M6">
+        <f>L6/(100*PI())</f>
+        <v>2.3863503245364119E-2</v>
+      </c>
       <c r="P6">
         <v>0.4</v>
       </c>
@@ -5868,6 +5872,10 @@
       <c r="L9">
         <f xml:space="preserve"> L8 * SIN( ATAN(L4))</f>
         <v>3.747918401171829</v>
+      </c>
+      <c r="M9">
+        <f>L9 / (100*PI())</f>
+        <v>1.1929994797031395E-2</v>
       </c>
       <c r="P9">
         <v>0.7</v>

</xml_diff>